<commit_message>
Add code to swap out non-matching team names
</commit_message>
<xml_diff>
--- a/NCAA Bracket Spreadsheet-copy.xlsx
+++ b/NCAA Bracket Spreadsheet-copy.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="602">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="618">
   <si>
     <t>Offensive</t>
   </si>
@@ -138,6 +138,12 @@
     <t>0.316</t>
   </si>
   <si>
+    <t>120.7</t>
+  </si>
+  <si>
+    <t>92.5</t>
+  </si>
+  <si>
     <t xml:space="preserve">12.7 </t>
   </si>
   <si>
@@ -165,9 +171,6 @@
     <t>122.4</t>
   </si>
   <si>
-    <t>92.5</t>
-  </si>
-  <si>
     <t xml:space="preserve">10.5 </t>
   </si>
   <si>
@@ -264,6 +267,12 @@
     <t>0.425</t>
   </si>
   <si>
+    <t>116.5</t>
+  </si>
+  <si>
+    <t>89.4</t>
+  </si>
+  <si>
     <t xml:space="preserve">11.8 </t>
   </si>
   <si>
@@ -327,9 +336,6 @@
     <t>116.9</t>
   </si>
   <si>
-    <t>89.4</t>
-  </si>
-  <si>
     <t xml:space="preserve">11.5 </t>
   </si>
   <si>
@@ -591,6 +597,12 @@
     <t>0.256</t>
   </si>
   <si>
+    <t>119.7</t>
+  </si>
+  <si>
+    <t>96.3</t>
+  </si>
+  <si>
     <t xml:space="preserve">12.3 </t>
   </si>
   <si>
@@ -669,6 +681,12 @@
     <t>0.246</t>
   </si>
   <si>
+    <t>119.8</t>
+  </si>
+  <si>
+    <t>95.0</t>
+  </si>
+  <si>
     <t xml:space="preserve">6.4 </t>
   </si>
   <si>
@@ -930,6 +948,12 @@
     <t>0.445</t>
   </si>
   <si>
+    <t>108.9</t>
+  </si>
+  <si>
+    <t>88.1</t>
+  </si>
+  <si>
     <t xml:space="preserve">9.1 </t>
   </si>
   <si>
@@ -1083,6 +1107,12 @@
     <t>0.287</t>
   </si>
   <si>
+    <t>109.9</t>
+  </si>
+  <si>
+    <t>94.8</t>
+  </si>
+  <si>
     <t xml:space="preserve">9.7 </t>
   </si>
   <si>
@@ -1155,6 +1185,9 @@
     <t>0.309</t>
   </si>
   <si>
+    <t>114.5</t>
+  </si>
+  <si>
     <t>Wake Forest</t>
   </si>
   <si>
@@ -1209,9 +1242,6 @@
     <t>111.9</t>
   </si>
   <si>
-    <t>96.3</t>
-  </si>
-  <si>
     <t xml:space="preserve">4.7 </t>
   </si>
   <si>
@@ -1350,6 +1380,12 @@
     <t>0.273</t>
   </si>
   <si>
+    <t>117.4</t>
+  </si>
+  <si>
+    <t>103.6</t>
+  </si>
+  <si>
     <t xml:space="preserve">8.6 </t>
   </si>
   <si>
@@ -1566,6 +1602,9 @@
     <t>0.382</t>
   </si>
   <si>
+    <t>97.3</t>
+  </si>
+  <si>
     <t xml:space="preserve">1.3 </t>
   </si>
   <si>
@@ -1650,9 +1689,6 @@
     <t>108.8</t>
   </si>
   <si>
-    <t>97.3</t>
-  </si>
-  <si>
     <t xml:space="preserve">7.0 </t>
   </si>
   <si>
@@ -1671,6 +1707,12 @@
     <t>74.4%</t>
   </si>
   <si>
+    <t>118.0</t>
+  </si>
+  <si>
+    <t>105.6</t>
+  </si>
+  <si>
     <t xml:space="preserve">1.7 </t>
   </si>
   <si>
@@ -1684,6 +1726,12 @@
   </si>
   <si>
     <t>0.294</t>
+  </si>
+  <si>
+    <t>111.1</t>
+  </si>
+  <si>
+    <t>100.9</t>
   </si>
   <si>
     <t xml:space="preserve">6.7 </t>
@@ -2913,17 +2961,17 @@
       <c r="J4" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="K4" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" s="61" t="n">
-        <v>0</v>
+      <c r="K4" s="61" t="s">
+        <v>38</v>
+      </c>
+      <c r="L4" s="61" t="s">
+        <v>39</v>
       </c>
       <c r="M4" s="61" t="n">
-        <v>0</v>
+        <v>28.2</v>
       </c>
       <c r="N4" s="61" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="O4" s="71" t="n"/>
     </row>
@@ -2932,43 +2980,43 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C5" s="61" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D5" s="61" t="s">
         <v>23</v>
       </c>
       <c r="E5" s="61" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F5" s="32" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G5" s="61" t="s">
         <v>34</v>
       </c>
       <c r="H5" s="61" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I5" s="61" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="J5" s="32" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="K5" s="61" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="L5" s="61" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="M5" s="61" t="n">
         <v>29.9</v>
       </c>
       <c r="N5" s="61" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:18">
@@ -2976,43 +3024,43 @@
         <v>4</v>
       </c>
       <c r="B6" s="61" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C6" s="61" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D6" s="61" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E6" s="61" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F6" s="32" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G6" s="61" t="s">
         <v>34</v>
       </c>
       <c r="H6" s="61" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I6" s="61" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J6" s="32" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="K6" s="61" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="L6" s="61" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="M6" s="61" t="n">
         <v>27.5</v>
       </c>
       <c r="N6" s="61" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:18">
@@ -3020,43 +3068,43 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C7" s="61" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D7" s="61" t="s">
         <v>31</v>
       </c>
       <c r="E7" s="61" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F7" s="32" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G7" s="61" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H7" s="61" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I7" s="61" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J7" s="32" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="K7" s="61" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="L7" s="61" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="M7" s="61" t="n">
         <v>27.7</v>
       </c>
       <c r="N7" s="61" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:18">
@@ -3064,43 +3112,43 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C8" s="61" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D8" s="61" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E8" s="61" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F8" s="32" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G8" s="61" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H8" s="61" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I8" s="61" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="J8" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="K8" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="L8" s="61" t="n">
-        <v>0</v>
+        <v>80</v>
+      </c>
+      <c r="K8" s="61" t="s">
+        <v>81</v>
+      </c>
+      <c r="L8" s="61" t="s">
+        <v>82</v>
       </c>
       <c r="M8" s="61" t="n">
-        <v>0</v>
+        <v>27.1</v>
       </c>
       <c r="N8" s="61" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:18">
@@ -3108,43 +3156,43 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C9" s="61" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D9" s="61" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E9" s="61" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="F9" s="32" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="G9" s="61" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H9" s="61" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="I9" s="61" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="J9" s="32" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="K9" s="61" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="L9" s="61" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="M9" s="61" t="n">
         <v>24.1</v>
       </c>
       <c r="N9" s="61" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:18">
@@ -3152,43 +3200,43 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C10" s="61" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D10" s="61" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="E10" s="61" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F10" s="32" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="G10" s="61" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="H10" s="61" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="I10" s="61" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="J10" s="32" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="K10" s="61" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="L10" s="61" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="M10" s="61" t="n">
         <v>27.5</v>
       </c>
       <c r="N10" s="61" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:18">
@@ -3196,43 +3244,43 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C11" s="61" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D11" s="61" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E11" s="61" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F11" s="32" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G11" s="61" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="H11" s="61" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="I11" s="61" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="J11" s="32" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="K11" s="61" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="L11" s="61" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="M11" s="61" t="n">
         <v>25.5</v>
       </c>
       <c r="N11" s="61" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="O11" s="23" t="n"/>
     </row>
@@ -3241,43 +3289,43 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C12" s="61" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D12" s="61" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E12" s="61" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="F12" s="32" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="G12" s="61" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="H12" s="61" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="I12" s="61" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="J12" s="32" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="K12" s="61" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="L12" s="61" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="M12" s="61" t="n">
         <v>25</v>
       </c>
       <c r="N12" s="61" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:18">
@@ -3285,43 +3333,43 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C13" s="61" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D13" s="61" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="E13" s="61" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="F13" s="32" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G13" s="61" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="H13" s="61" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="I13" s="61" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="J13" s="32" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="K13" s="61" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="L13" s="61" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="M13" s="61" t="n">
         <v>24.3</v>
       </c>
       <c r="N13" s="61" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="O13" s="23" t="n"/>
     </row>
@@ -3330,37 +3378,37 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C14" s="61" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D14" s="61" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E14" s="61" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F14" s="32" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="G14" s="61" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="H14" s="61" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="I14" s="61" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="J14" s="32" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="K14" s="61" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="L14" s="61" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="M14" s="61" t="n">
         <v>23.6</v>
@@ -3374,43 +3422,43 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C15" s="61" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D15" s="61" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="E15" s="61" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="F15" s="32" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="G15" s="61" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="H15" s="61" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="I15" s="61" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="J15" s="32" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="K15" s="61" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="L15" s="61" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="M15" s="61" t="n">
         <v>26.1</v>
       </c>
       <c r="N15" s="61" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="16" s="30" spans="1:18">
@@ -3418,43 +3466,43 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C16" s="61" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D16" s="61" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E16" s="61" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="F16" s="32" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="G16" s="61" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="H16" s="61" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="I16" s="61" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="J16" s="32" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="K16" s="61" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="L16" s="61" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="M16" s="61" t="n">
         <v>23.1</v>
       </c>
       <c r="N16" s="61" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="17" spans="1:18">
@@ -3462,43 +3510,43 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C17" s="61" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D17" s="61" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E17" s="61" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="F17" s="32" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G17" s="61" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="H17" s="61" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="I17" s="61" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="J17" s="32" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="K17" s="61" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="L17" s="61" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="M17" s="61" t="n">
         <v>23</v>
       </c>
       <c r="N17" s="61" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="18" spans="1:18">
@@ -3506,43 +3554,43 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C18" s="61" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D18" s="61" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="E18" s="61" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="F18" s="32" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="G18" s="61" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="H18" s="61" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="I18" s="61" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="J18" s="32" t="s">
-        <v>188</v>
-      </c>
-      <c r="K18" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="L18" s="61" t="n">
-        <v>0</v>
+        <v>190</v>
+      </c>
+      <c r="K18" s="61" t="s">
+        <v>191</v>
+      </c>
+      <c r="L18" s="61" t="s">
+        <v>192</v>
       </c>
       <c r="M18" s="61" t="n">
-        <v>0</v>
+        <v>23.4</v>
       </c>
       <c r="N18" s="61" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="O18" s="23" t="n"/>
     </row>
@@ -3551,43 +3599,43 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="C19" s="61" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="D19" s="61" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E19" s="61" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="F19" s="32" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="G19" s="61" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="H19" s="61" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="I19" s="61" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="J19" s="32" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="K19" s="61" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="L19" s="61" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="M19" s="61" t="n">
         <v>24.2</v>
       </c>
       <c r="N19" s="61" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
     </row>
     <row r="20" spans="1:18">
@@ -3595,43 +3643,43 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="C20" s="61" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="D20" s="61" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="E20" s="61" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="F20" s="32" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="G20" s="61" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="H20" s="61" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="I20" s="61" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="J20" s="32" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="K20" s="61" t="s">
         <v>26</v>
       </c>
       <c r="L20" s="61" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="M20" s="61" t="n">
         <v>23.3</v>
       </c>
       <c r="N20" s="61" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
     </row>
     <row r="21" s="30" spans="1:18">
@@ -3639,43 +3687,43 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="C21" s="61" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="D21" s="61" t="s">
         <v>19</v>
       </c>
       <c r="E21" s="61" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="F21" s="32" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G21" s="61" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="H21" s="61" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="I21" s="61" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="J21" s="32" t="s">
-        <v>214</v>
-      </c>
-      <c r="K21" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="L21" s="61" t="n">
-        <v>0</v>
+        <v>218</v>
+      </c>
+      <c r="K21" s="61" t="s">
+        <v>219</v>
+      </c>
+      <c r="L21" s="61" t="s">
+        <v>220</v>
       </c>
       <c r="M21" s="61" t="n">
-        <v>0</v>
+        <v>24.8</v>
       </c>
       <c r="N21" s="61" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
     </row>
     <row r="22" spans="1:18">
@@ -3683,43 +3731,43 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="C22" s="61" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="D22" s="61" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="E22" s="61" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="F22" s="32" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="G22" s="61" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="H22" s="61" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="I22" s="61" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="J22" s="32" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="K22" s="61" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="L22" s="61" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="M22" s="61" t="n">
         <v>22.2</v>
       </c>
       <c r="N22" s="61" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
     </row>
     <row r="23" spans="1:18">
@@ -3727,43 +3775,43 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="C23" s="61" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="D23" s="61" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="E23" s="61" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="F23" s="32" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="G23" s="61" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="H23" s="61" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="I23" s="61" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="J23" s="32" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="K23" s="61" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="L23" s="61" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="M23" s="61" t="n">
         <v>23</v>
       </c>
       <c r="N23" s="61" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="O23" s="23" t="n"/>
     </row>
@@ -3772,43 +3820,43 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="C24" s="61" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="D24" s="61" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="E24" s="61" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="F24" s="32" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="G24" s="61" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="H24" s="61" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="I24" s="61" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="J24" s="32" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="K24" s="61" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="L24" s="61" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="M24" s="61" t="n">
         <v>20.1</v>
       </c>
       <c r="N24" s="61" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
     </row>
     <row r="25" spans="1:18">
@@ -3816,43 +3864,43 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="C25" s="61" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="D25" s="61" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="E25" s="61" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="F25" s="32" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="G25" s="61" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="H25" s="61" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="I25" s="61" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="J25" s="32" t="s">
-        <v>254</v>
-      </c>
-      <c r="K25" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="L25" s="61" t="n">
-        <v>0</v>
+        <v>260</v>
+      </c>
+      <c r="K25" s="61" t="s">
+        <v>158</v>
+      </c>
+      <c r="L25" s="61" t="s">
+        <v>220</v>
       </c>
       <c r="M25" s="61" t="n">
-        <v>0</v>
+        <v>23.7</v>
       </c>
       <c r="N25" s="61" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
     </row>
     <row r="26" spans="1:18">
@@ -3860,43 +3908,43 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="C26" s="61" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="D26" s="61" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E26" s="61" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="F26" s="32" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="G26" s="61" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="H26" s="61" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="I26" s="61" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="J26" s="32" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
       <c r="K26" s="61" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="L26" s="61" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="M26" s="61" t="n">
         <v>20.7</v>
       </c>
       <c r="N26" s="61" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
     </row>
     <row r="27" spans="1:18">
@@ -3904,43 +3952,43 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
       <c r="C27" s="61" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="D27" s="61" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="E27" s="61" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="F27" s="32" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="G27" s="61" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="H27" s="61" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
       <c r="I27" s="61" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="J27" s="32" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="K27" s="61" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="L27" s="61" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="M27" s="61" t="n">
         <v>22.5</v>
       </c>
       <c r="N27" s="61" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="28" spans="1:18">
@@ -3948,43 +3996,43 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="C28" s="61" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="D28" s="61" t="s">
+        <v>286</v>
+      </c>
+      <c r="E28" s="61" t="s">
+        <v>287</v>
+      </c>
+      <c r="F28" s="32" t="s">
+        <v>209</v>
+      </c>
+      <c r="G28" s="61" t="s">
+        <v>288</v>
+      </c>
+      <c r="H28" s="61" t="s">
+        <v>55</v>
+      </c>
+      <c r="I28" s="61" t="s">
         <v>280</v>
       </c>
-      <c r="E28" s="61" t="s">
-        <v>281</v>
-      </c>
-      <c r="F28" s="32" t="s">
-        <v>205</v>
-      </c>
-      <c r="G28" s="61" t="s">
-        <v>282</v>
-      </c>
-      <c r="H28" s="61" t="s">
-        <v>54</v>
-      </c>
-      <c r="I28" s="61" t="s">
-        <v>274</v>
-      </c>
       <c r="J28" s="32" t="s">
-        <v>283</v>
+        <v>289</v>
       </c>
       <c r="K28" s="61" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
       <c r="L28" s="61" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="M28" s="61" t="n">
         <v>19.7</v>
       </c>
       <c r="N28" s="61" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
     </row>
     <row r="29" spans="1:18">
@@ -3992,37 +4040,37 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>286</v>
+        <v>292</v>
       </c>
       <c r="C29" s="61" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
       <c r="D29" s="61" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="E29" s="61" t="s">
-        <v>288</v>
+        <v>294</v>
       </c>
       <c r="F29" s="32" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
       <c r="G29" s="61" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="H29" s="61" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="I29" s="61" t="s">
-        <v>291</v>
+        <v>297</v>
       </c>
       <c r="J29" s="32" t="s">
-        <v>292</v>
+        <v>298</v>
       </c>
       <c r="K29" s="61" t="s">
-        <v>293</v>
+        <v>299</v>
       </c>
       <c r="L29" s="61" t="s">
-        <v>294</v>
+        <v>300</v>
       </c>
       <c r="M29" s="61" t="n">
         <v>18.8</v>
@@ -4036,43 +4084,43 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
       <c r="C30" s="61" t="s">
-        <v>296</v>
+        <v>302</v>
       </c>
       <c r="D30" s="61" t="s">
-        <v>297</v>
+        <v>303</v>
       </c>
       <c r="E30" s="61" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="F30" s="32" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="G30" s="61" t="s">
-        <v>298</v>
+        <v>304</v>
       </c>
       <c r="H30" s="61" t="s">
-        <v>299</v>
+        <v>305</v>
       </c>
       <c r="I30" s="61" t="s">
-        <v>300</v>
+        <v>306</v>
       </c>
       <c r="J30" s="32" t="s">
-        <v>301</v>
-      </c>
-      <c r="K30" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="L30" s="61" t="n">
-        <v>0</v>
+        <v>307</v>
+      </c>
+      <c r="K30" s="61" t="s">
+        <v>308</v>
+      </c>
+      <c r="L30" s="61" t="s">
+        <v>309</v>
       </c>
       <c r="M30" s="61" t="n">
-        <v>0</v>
+        <v>20.8</v>
       </c>
       <c r="N30" s="61" t="s">
-        <v>302</v>
+        <v>310</v>
       </c>
     </row>
     <row r="31" spans="1:18">
@@ -4080,43 +4128,43 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>303</v>
+        <v>311</v>
       </c>
       <c r="C31" s="61" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="D31" s="61" t="s">
-        <v>304</v>
+        <v>312</v>
       </c>
       <c r="E31" s="61" t="s">
-        <v>305</v>
+        <v>313</v>
       </c>
       <c r="F31" s="32" t="s">
-        <v>306</v>
+        <v>314</v>
       </c>
       <c r="G31" s="61" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="H31" s="61" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="I31" s="61" t="s">
         <v>36</v>
       </c>
       <c r="J31" s="32" t="s">
-        <v>307</v>
+        <v>315</v>
       </c>
       <c r="K31" s="61" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="L31" s="61" t="s">
-        <v>309</v>
+        <v>317</v>
       </c>
       <c r="M31" s="61" t="n">
         <v>16.7</v>
       </c>
       <c r="N31" s="61" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
     </row>
     <row r="32" spans="1:18">
@@ -4124,43 +4172,43 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>310</v>
+        <v>318</v>
       </c>
       <c r="C32" s="61" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
       <c r="D32" s="61" t="s">
-        <v>311</v>
+        <v>319</v>
       </c>
       <c r="E32" s="61" t="s">
-        <v>312</v>
+        <v>320</v>
       </c>
       <c r="F32" s="32" t="s">
-        <v>313</v>
+        <v>321</v>
       </c>
       <c r="G32" s="61" t="s">
-        <v>314</v>
+        <v>322</v>
       </c>
       <c r="H32" s="61" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="I32" s="61" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="J32" s="32" t="s">
-        <v>315</v>
+        <v>323</v>
       </c>
       <c r="K32" s="61" t="s">
-        <v>316</v>
+        <v>324</v>
       </c>
       <c r="L32" s="61" t="s">
-        <v>317</v>
+        <v>325</v>
       </c>
       <c r="M32" s="61" t="n">
         <v>16.6</v>
       </c>
       <c r="N32" s="61" t="s">
-        <v>318</v>
+        <v>326</v>
       </c>
     </row>
     <row r="33" spans="1:18">
@@ -4168,43 +4216,43 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>319</v>
+        <v>327</v>
       </c>
       <c r="C33" s="61" t="s">
-        <v>320</v>
+        <v>328</v>
       </c>
       <c r="D33" s="61" t="s">
-        <v>321</v>
+        <v>329</v>
       </c>
       <c r="E33" s="61" t="s">
-        <v>322</v>
+        <v>330</v>
       </c>
       <c r="F33" s="32" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="G33" s="61" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="H33" s="61" t="s">
-        <v>323</v>
+        <v>331</v>
       </c>
       <c r="I33" s="61" t="s">
-        <v>324</v>
+        <v>332</v>
       </c>
       <c r="J33" s="32" t="s">
-        <v>325</v>
+        <v>333</v>
       </c>
       <c r="K33" s="61" t="s">
-        <v>326</v>
+        <v>334</v>
       </c>
       <c r="L33" s="61" t="s">
-        <v>327</v>
+        <v>335</v>
       </c>
       <c r="M33" s="61" t="n">
         <v>14.5</v>
       </c>
       <c r="N33" s="61" t="s">
-        <v>328</v>
+        <v>336</v>
       </c>
     </row>
     <row r="34" spans="1:18">
@@ -4212,43 +4260,43 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>329</v>
+        <v>337</v>
       </c>
       <c r="C34" s="61" t="s">
-        <v>330</v>
+        <v>338</v>
       </c>
       <c r="D34" s="61" t="s">
-        <v>297</v>
+        <v>303</v>
       </c>
       <c r="E34" s="61" t="s">
-        <v>331</v>
+        <v>339</v>
       </c>
       <c r="F34" s="32" t="s">
-        <v>332</v>
+        <v>340</v>
       </c>
       <c r="G34" s="61" t="s">
-        <v>333</v>
+        <v>341</v>
       </c>
       <c r="H34" s="61" t="s">
-        <v>334</v>
+        <v>342</v>
       </c>
       <c r="I34" s="61" t="s">
-        <v>335</v>
+        <v>343</v>
       </c>
       <c r="J34" s="32" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="K34" s="61" t="s">
-        <v>336</v>
+        <v>344</v>
       </c>
       <c r="L34" s="61" t="s">
-        <v>337</v>
+        <v>345</v>
       </c>
       <c r="M34" s="61" t="n">
         <v>13.3</v>
       </c>
       <c r="N34" s="61" t="s">
-        <v>338</v>
+        <v>346</v>
       </c>
     </row>
     <row r="35" spans="1:18">
@@ -4256,43 +4304,43 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>339</v>
+        <v>347</v>
       </c>
       <c r="C35" s="61" t="s">
-        <v>340</v>
+        <v>348</v>
       </c>
       <c r="D35" s="61" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E35" s="61" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F35" s="32" t="s">
-        <v>341</v>
+        <v>349</v>
       </c>
       <c r="G35" s="61" t="s">
-        <v>342</v>
+        <v>350</v>
       </c>
       <c r="H35" s="61" t="s">
-        <v>343</v>
+        <v>351</v>
       </c>
       <c r="I35" s="61" t="s">
-        <v>344</v>
+        <v>352</v>
       </c>
       <c r="J35" s="32" t="s">
-        <v>307</v>
+        <v>315</v>
       </c>
       <c r="K35" s="61" t="s">
-        <v>345</v>
+        <v>353</v>
       </c>
       <c r="L35" s="61" t="s">
-        <v>346</v>
+        <v>354</v>
       </c>
       <c r="M35" s="61" t="n">
         <v>17.4</v>
       </c>
       <c r="N35" s="61" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="36" spans="1:18">
@@ -4300,43 +4348,43 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>347</v>
+        <v>355</v>
       </c>
       <c r="C36" s="61" t="s">
-        <v>348</v>
+        <v>356</v>
       </c>
       <c r="D36" s="61" t="s">
-        <v>349</v>
+        <v>357</v>
       </c>
       <c r="E36" s="61" t="s">
-        <v>350</v>
+        <v>358</v>
       </c>
       <c r="F36" s="32" t="s">
         <v>33</v>
       </c>
       <c r="G36" s="61" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="H36" s="61" t="s">
-        <v>351</v>
+        <v>359</v>
       </c>
       <c r="I36" s="61" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="J36" s="32" t="s">
-        <v>352</v>
-      </c>
-      <c r="K36" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="L36" s="61" t="n">
-        <v>0</v>
+        <v>360</v>
+      </c>
+      <c r="K36" s="61" t="s">
+        <v>361</v>
+      </c>
+      <c r="L36" s="61" t="s">
+        <v>362</v>
       </c>
       <c r="M36" s="61" t="n">
-        <v>0</v>
+        <v>15.1</v>
       </c>
       <c r="N36" s="61" t="s">
-        <v>353</v>
+        <v>363</v>
       </c>
     </row>
     <row r="37" spans="1:18">
@@ -4344,43 +4392,43 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>354</v>
+        <v>364</v>
       </c>
       <c r="C37" s="61" t="s">
-        <v>355</v>
+        <v>365</v>
       </c>
       <c r="D37" s="61" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="E37" s="61" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="F37" s="32" t="s">
-        <v>356</v>
+        <v>366</v>
       </c>
       <c r="G37" s="61" t="s">
-        <v>357</v>
+        <v>367</v>
       </c>
       <c r="H37" s="61" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="I37" s="61" t="s">
-        <v>358</v>
+        <v>368</v>
       </c>
       <c r="J37" s="32" t="s">
-        <v>359</v>
+        <v>369</v>
       </c>
       <c r="K37" s="61" t="s">
-        <v>360</v>
+        <v>370</v>
       </c>
       <c r="L37" s="61" t="s">
-        <v>361</v>
+        <v>371</v>
       </c>
       <c r="M37" s="61" t="n">
         <v>16.3</v>
       </c>
       <c r="N37" s="61" t="s">
-        <v>362</v>
+        <v>372</v>
       </c>
     </row>
     <row r="38" spans="1:18">
@@ -4388,43 +4436,43 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>363</v>
+        <v>373</v>
       </c>
       <c r="C38" s="61" t="s">
+        <v>274</v>
+      </c>
+      <c r="D38" s="61" t="s">
+        <v>374</v>
+      </c>
+      <c r="E38" s="61" t="s">
+        <v>375</v>
+      </c>
+      <c r="F38" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="G38" s="61" t="s">
+        <v>376</v>
+      </c>
+      <c r="H38" s="61" t="s">
+        <v>377</v>
+      </c>
+      <c r="I38" s="61" t="s">
         <v>268</v>
       </c>
-      <c r="D38" s="61" t="s">
-        <v>364</v>
-      </c>
-      <c r="E38" s="61" t="s">
-        <v>365</v>
-      </c>
-      <c r="F38" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="G38" s="61" t="s">
-        <v>366</v>
-      </c>
-      <c r="H38" s="61" t="s">
-        <v>367</v>
-      </c>
-      <c r="I38" s="61" t="s">
-        <v>262</v>
-      </c>
       <c r="J38" s="32" t="s">
-        <v>368</v>
+        <v>378</v>
       </c>
       <c r="K38" s="61" t="s">
-        <v>369</v>
+        <v>379</v>
       </c>
       <c r="L38" s="61" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="M38" s="61" t="n">
         <v>15.5</v>
       </c>
       <c r="N38" s="61" t="s">
-        <v>353</v>
+        <v>363</v>
       </c>
     </row>
     <row r="39" spans="1:18">
@@ -4432,43 +4480,43 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>371</v>
+        <v>381</v>
       </c>
       <c r="C39" s="61" t="s">
-        <v>340</v>
+        <v>348</v>
       </c>
       <c r="D39" s="61" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E39" s="61" t="s">
-        <v>372</v>
+        <v>382</v>
       </c>
       <c r="F39" s="32" t="s">
-        <v>373</v>
+        <v>383</v>
       </c>
       <c r="G39" s="61" t="s">
-        <v>333</v>
+        <v>341</v>
       </c>
       <c r="H39" s="61" t="s">
-        <v>374</v>
+        <v>384</v>
       </c>
       <c r="I39" s="61" t="s">
-        <v>375</v>
+        <v>385</v>
       </c>
       <c r="J39" s="32" t="s">
-        <v>376</v>
-      </c>
-      <c r="K39" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="L39" s="61" t="n">
-        <v>0</v>
+        <v>386</v>
+      </c>
+      <c r="K39" s="61" t="s">
+        <v>387</v>
+      </c>
+      <c r="L39" s="61" t="s">
+        <v>271</v>
       </c>
       <c r="M39" s="61" t="n">
-        <v>0</v>
+        <v>17.5</v>
       </c>
       <c r="N39" s="61" t="s">
-        <v>328</v>
+        <v>336</v>
       </c>
     </row>
     <row r="40" spans="1:18">
@@ -4476,43 +4524,43 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>377</v>
+        <v>388</v>
       </c>
       <c r="C40" s="61" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D40" s="61" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E40" s="61" t="s">
-        <v>378</v>
+        <v>389</v>
       </c>
       <c r="F40" s="32" t="s">
-        <v>379</v>
+        <v>390</v>
       </c>
       <c r="G40" s="61" t="s">
-        <v>340</v>
+        <v>348</v>
       </c>
       <c r="H40" s="61" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="I40" s="61" t="s">
-        <v>380</v>
+        <v>391</v>
       </c>
       <c r="J40" s="32" t="s">
-        <v>381</v>
+        <v>392</v>
       </c>
       <c r="K40" s="61" t="s">
-        <v>382</v>
+        <v>393</v>
       </c>
       <c r="L40" s="61" t="s">
-        <v>383</v>
+        <v>394</v>
       </c>
       <c r="M40" s="61" t="n">
         <v>16.3</v>
       </c>
       <c r="N40" s="61" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="41" spans="1:18">
@@ -4520,43 +4568,43 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>384</v>
+        <v>395</v>
       </c>
       <c r="C41" s="61" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D41" s="61" t="s">
+        <v>377</v>
+      </c>
+      <c r="E41" s="61" t="s">
+        <v>396</v>
+      </c>
+      <c r="F41" s="32" t="s">
+        <v>397</v>
+      </c>
+      <c r="G41" s="61" t="s">
         <v>367</v>
       </c>
-      <c r="E41" s="61" t="s">
-        <v>385</v>
-      </c>
-      <c r="F41" s="32" t="s">
-        <v>386</v>
-      </c>
-      <c r="G41" s="61" t="s">
-        <v>357</v>
-      </c>
       <c r="H41" s="61" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I41" s="61" t="s">
-        <v>358</v>
+        <v>368</v>
       </c>
       <c r="J41" s="32" t="s">
-        <v>292</v>
+        <v>298</v>
       </c>
       <c r="K41" s="61" t="s">
-        <v>387</v>
+        <v>398</v>
       </c>
       <c r="L41" s="61" t="s">
-        <v>388</v>
+        <v>399</v>
       </c>
       <c r="M41" s="61" t="n">
         <v>16</v>
       </c>
       <c r="N41" s="61" t="s">
-        <v>389</v>
+        <v>400</v>
       </c>
     </row>
     <row r="42" spans="1:18">
@@ -4564,43 +4612,43 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>390</v>
+        <v>401</v>
       </c>
       <c r="C42" s="61" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="D42" s="61" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="E42" s="61" t="s">
-        <v>391</v>
+        <v>402</v>
       </c>
       <c r="F42" s="32" t="s">
-        <v>392</v>
+        <v>403</v>
       </c>
       <c r="G42" s="61" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="H42" s="61" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="I42" s="61" t="s">
-        <v>393</v>
+        <v>404</v>
       </c>
       <c r="J42" s="32" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="K42" s="61" t="s">
-        <v>394</v>
+        <v>405</v>
       </c>
       <c r="L42" s="61" t="s">
-        <v>395</v>
+        <v>192</v>
       </c>
       <c r="M42" s="61" t="n">
         <v>15.6</v>
       </c>
       <c r="N42" s="61" t="s">
-        <v>396</v>
+        <v>406</v>
       </c>
     </row>
     <row r="43" spans="1:18">
@@ -4608,43 +4656,43 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>397</v>
+        <v>407</v>
       </c>
       <c r="C43" s="61" t="s">
-        <v>398</v>
+        <v>408</v>
       </c>
       <c r="D43" s="61" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="E43" s="61" t="s">
-        <v>399</v>
+        <v>409</v>
       </c>
       <c r="F43" s="32" t="s">
         <v>33</v>
       </c>
       <c r="G43" s="61" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="H43" s="61" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="I43" s="61" t="s">
-        <v>400</v>
+        <v>410</v>
       </c>
       <c r="J43" s="32" t="s">
-        <v>401</v>
+        <v>411</v>
       </c>
       <c r="K43" s="61" t="s">
-        <v>402</v>
+        <v>412</v>
       </c>
       <c r="L43" s="61" t="s">
-        <v>403</v>
+        <v>413</v>
       </c>
       <c r="M43" s="61" t="n">
         <v>14.4</v>
       </c>
       <c r="N43" s="61" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="44" spans="1:18">
@@ -4652,43 +4700,43 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>404</v>
+        <v>414</v>
       </c>
       <c r="C44" s="61" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D44" s="61" t="s">
-        <v>374</v>
+        <v>384</v>
       </c>
       <c r="E44" s="61" t="s">
-        <v>391</v>
+        <v>402</v>
       </c>
       <c r="F44" s="32" t="s">
-        <v>405</v>
+        <v>415</v>
       </c>
       <c r="G44" s="61" t="s">
         <v>34</v>
       </c>
       <c r="H44" s="61" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I44" s="61" t="s">
-        <v>324</v>
+        <v>332</v>
       </c>
       <c r="J44" s="32" t="s">
-        <v>406</v>
+        <v>416</v>
       </c>
       <c r="K44" s="61" t="s">
-        <v>407</v>
+        <v>417</v>
       </c>
       <c r="L44" s="61" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="M44" s="61" t="n">
         <v>16.5</v>
       </c>
       <c r="N44" s="61" t="s">
-        <v>328</v>
+        <v>336</v>
       </c>
     </row>
     <row r="45" spans="1:18">
@@ -4696,43 +4744,43 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>408</v>
+        <v>418</v>
       </c>
       <c r="C45" s="61" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D45" s="61" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E45" s="61" t="s">
-        <v>399</v>
+        <v>409</v>
       </c>
       <c r="F45" s="32" t="s">
-        <v>409</v>
+        <v>419</v>
       </c>
       <c r="G45" s="61" t="s">
-        <v>410</v>
+        <v>420</v>
       </c>
       <c r="H45" s="61" t="s">
-        <v>304</v>
+        <v>312</v>
       </c>
       <c r="I45" s="61" t="s">
-        <v>411</v>
+        <v>421</v>
       </c>
       <c r="J45" s="32" t="s">
         <v>21</v>
       </c>
       <c r="K45" s="61" t="s">
-        <v>326</v>
+        <v>334</v>
       </c>
       <c r="L45" s="61" t="s">
-        <v>412</v>
+        <v>422</v>
       </c>
       <c r="M45" s="61" t="n">
         <v>16.3</v>
       </c>
       <c r="N45" s="61" t="s">
-        <v>389</v>
+        <v>400</v>
       </c>
     </row>
     <row r="46" spans="1:18">
@@ -4740,43 +4788,43 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>413</v>
+        <v>423</v>
       </c>
       <c r="C46" s="61" t="s">
-        <v>414</v>
+        <v>424</v>
       </c>
       <c r="D46" s="61" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="E46" s="61" t="s">
-        <v>415</v>
+        <v>425</v>
       </c>
       <c r="F46" s="32" t="s">
-        <v>315</v>
+        <v>323</v>
       </c>
       <c r="G46" s="61" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="H46" s="61" t="s">
-        <v>416</v>
+        <v>426</v>
       </c>
       <c r="I46" s="61" t="s">
-        <v>417</v>
+        <v>427</v>
       </c>
       <c r="J46" s="32" t="s">
-        <v>315</v>
+        <v>323</v>
       </c>
       <c r="K46" s="61" t="s">
-        <v>418</v>
+        <v>428</v>
       </c>
       <c r="L46" s="61" t="s">
-        <v>419</v>
+        <v>429</v>
       </c>
       <c r="M46" s="61" t="n">
         <v>15.2</v>
       </c>
       <c r="N46" s="61" t="s">
-        <v>420</v>
+        <v>430</v>
       </c>
     </row>
     <row r="47" spans="1:18">
@@ -4784,43 +4832,43 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>421</v>
+        <v>431</v>
       </c>
       <c r="C47" s="61" t="s">
-        <v>422</v>
+        <v>432</v>
       </c>
       <c r="D47" s="61" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="E47" s="61" t="s">
-        <v>423</v>
+        <v>433</v>
       </c>
       <c r="F47" s="32" t="s">
-        <v>424</v>
+        <v>434</v>
       </c>
       <c r="G47" s="61" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="H47" s="61" t="s">
-        <v>425</v>
+        <v>435</v>
       </c>
       <c r="I47" s="61" t="s">
-        <v>426</v>
+        <v>436</v>
       </c>
       <c r="J47" s="32" t="s">
-        <v>427</v>
+        <v>437</v>
       </c>
       <c r="K47" s="61" t="s">
-        <v>428</v>
+        <v>438</v>
       </c>
       <c r="L47" s="61" t="s">
-        <v>429</v>
+        <v>439</v>
       </c>
       <c r="M47" s="61" t="n">
         <v>15.8</v>
       </c>
       <c r="N47" s="61" t="s">
-        <v>430</v>
+        <v>440</v>
       </c>
     </row>
     <row r="48" spans="1:18">
@@ -4828,43 +4876,43 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>431</v>
+        <v>441</v>
       </c>
       <c r="C48" s="61" t="s">
-        <v>348</v>
+        <v>356</v>
       </c>
       <c r="D48" s="61" t="s">
-        <v>425</v>
+        <v>435</v>
       </c>
       <c r="E48" s="61" t="s">
-        <v>432</v>
+        <v>442</v>
       </c>
       <c r="F48" s="32" t="s">
-        <v>433</v>
+        <v>443</v>
       </c>
       <c r="G48" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="H48" s="61" t="s">
+        <v>444</v>
+      </c>
+      <c r="I48" s="61" t="s">
+        <v>46</v>
+      </c>
+      <c r="J48" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="H48" s="61" t="s">
-        <v>434</v>
-      </c>
-      <c r="I48" s="61" t="s">
-        <v>44</v>
-      </c>
-      <c r="J48" s="32" t="s">
-        <v>63</v>
-      </c>
       <c r="K48" s="61" t="s">
-        <v>435</v>
+        <v>445</v>
       </c>
       <c r="L48" s="61" t="s">
-        <v>436</v>
+        <v>446</v>
       </c>
       <c r="M48" s="61" t="n">
         <v>14.1</v>
       </c>
       <c r="N48" s="61" t="s">
-        <v>437</v>
+        <v>447</v>
       </c>
     </row>
     <row r="49" spans="1:18">
@@ -4872,43 +4920,43 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>438</v>
+        <v>448</v>
       </c>
       <c r="C49" s="61" t="s">
-        <v>439</v>
+        <v>449</v>
       </c>
       <c r="D49" s="61" t="s">
-        <v>311</v>
+        <v>319</v>
       </c>
       <c r="E49" s="61" t="s">
-        <v>299</v>
+        <v>305</v>
       </c>
       <c r="F49" s="32" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G49" s="61" t="s">
-        <v>348</v>
+        <v>356</v>
       </c>
       <c r="H49" s="61" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="I49" s="61" t="s">
-        <v>440</v>
+        <v>450</v>
       </c>
       <c r="J49" s="32" t="s">
-        <v>441</v>
-      </c>
-      <c r="K49" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="L49" s="61" t="n">
-        <v>0</v>
+        <v>451</v>
+      </c>
+      <c r="K49" s="61" t="s">
+        <v>452</v>
+      </c>
+      <c r="L49" s="61" t="s">
+        <v>453</v>
       </c>
       <c r="M49" s="61" t="n">
-        <v>0</v>
+        <v>13.8</v>
       </c>
       <c r="N49" s="61" t="s">
-        <v>442</v>
+        <v>454</v>
       </c>
     </row>
     <row r="50" spans="1:18">
@@ -4916,43 +4964,43 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>443</v>
+        <v>455</v>
       </c>
       <c r="C50" s="61" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D50" s="61" t="s">
-        <v>334</v>
+        <v>342</v>
       </c>
       <c r="E50" s="61" t="s">
-        <v>423</v>
+        <v>433</v>
       </c>
       <c r="F50" s="32" t="s">
-        <v>444</v>
+        <v>456</v>
       </c>
       <c r="G50" s="61" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H50" s="61" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="I50" s="61" t="s">
-        <v>445</v>
+        <v>457</v>
       </c>
       <c r="J50" s="32" t="s">
-        <v>446</v>
+        <v>458</v>
       </c>
       <c r="K50" s="61" t="s">
-        <v>447</v>
+        <v>459</v>
       </c>
       <c r="L50" s="61" t="s">
-        <v>448</v>
+        <v>460</v>
       </c>
       <c r="M50" s="61" t="n">
         <v>14.3</v>
       </c>
       <c r="N50" s="61" t="s">
-        <v>449</v>
+        <v>461</v>
       </c>
     </row>
     <row r="51" spans="1:18">
@@ -4960,43 +5008,43 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>450</v>
+        <v>462</v>
       </c>
       <c r="C51" s="61" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="D51" s="61" t="s">
         <v>35</v>
       </c>
       <c r="E51" s="61" t="s">
-        <v>451</v>
+        <v>463</v>
       </c>
       <c r="F51" s="32" t="s">
-        <v>452</v>
+        <v>464</v>
       </c>
       <c r="G51" s="61" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="H51" s="61" t="s">
-        <v>311</v>
+        <v>319</v>
       </c>
       <c r="I51" s="61" t="s">
-        <v>453</v>
+        <v>465</v>
       </c>
       <c r="J51" s="32" t="s">
-        <v>454</v>
+        <v>466</v>
       </c>
       <c r="K51" s="61" t="s">
-        <v>455</v>
+        <v>467</v>
       </c>
       <c r="L51" s="61" t="s">
-        <v>456</v>
+        <v>468</v>
       </c>
       <c r="M51" s="61" t="n">
         <v>13.7</v>
       </c>
       <c r="N51" s="61" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
     </row>
     <row r="52" spans="1:18">
@@ -5004,43 +5052,43 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>457</v>
+        <v>469</v>
       </c>
       <c r="C52" s="61" t="s">
-        <v>458</v>
+        <v>470</v>
       </c>
       <c r="D52" s="61" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E52" s="61" t="s">
-        <v>459</v>
+        <v>471</v>
       </c>
       <c r="F52" s="32" t="s">
-        <v>460</v>
+        <v>472</v>
       </c>
       <c r="G52" s="61" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="H52" s="61" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I52" s="61" t="s">
-        <v>461</v>
+        <v>473</v>
       </c>
       <c r="J52" s="32" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="K52" s="61" t="s">
-        <v>462</v>
+        <v>474</v>
       </c>
       <c r="L52" s="61" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="M52" s="61" t="n">
         <v>14.2</v>
       </c>
       <c r="N52" s="61" t="s">
-        <v>463</v>
+        <v>475</v>
       </c>
     </row>
     <row r="53" spans="1:18">
@@ -5048,43 +5096,43 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>464</v>
+        <v>476</v>
       </c>
       <c r="C53" s="61" t="s">
         <v>34</v>
       </c>
       <c r="D53" s="61" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="E53" s="61" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="F53" s="32" t="s">
-        <v>465</v>
+        <v>477</v>
       </c>
       <c r="G53" s="61" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="H53" s="61" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="I53" s="61" t="s">
-        <v>466</v>
+        <v>478</v>
       </c>
       <c r="J53" s="32" t="s">
-        <v>467</v>
+        <v>479</v>
       </c>
       <c r="K53" s="61" t="s">
-        <v>468</v>
+        <v>480</v>
       </c>
       <c r="L53" s="61" t="s">
-        <v>469</v>
+        <v>481</v>
       </c>
       <c r="M53" s="61" t="n">
         <v>12.2</v>
       </c>
       <c r="N53" s="61" t="s">
-        <v>470</v>
+        <v>482</v>
       </c>
     </row>
     <row r="54" spans="1:18">
@@ -5092,43 +5140,43 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>471</v>
+        <v>483</v>
       </c>
       <c r="C54" s="61" t="s">
         <v>30</v>
       </c>
       <c r="D54" s="61" t="s">
-        <v>472</v>
+        <v>484</v>
       </c>
       <c r="E54" s="61" t="s">
-        <v>473</v>
+        <v>485</v>
       </c>
       <c r="F54" s="32" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="G54" s="61" t="s">
+        <v>486</v>
+      </c>
+      <c r="H54" s="61" t="s">
+        <v>487</v>
+      </c>
+      <c r="I54" s="61" t="s">
+        <v>488</v>
+      </c>
+      <c r="J54" s="32" t="s">
+        <v>489</v>
+      </c>
+      <c r="K54" s="61" t="s">
         <v>474</v>
       </c>
-      <c r="H54" s="61" t="s">
-        <v>475</v>
-      </c>
-      <c r="I54" s="61" t="s">
-        <v>476</v>
-      </c>
-      <c r="J54" s="32" t="s">
-        <v>477</v>
-      </c>
-      <c r="K54" s="61" t="s">
-        <v>462</v>
-      </c>
       <c r="L54" s="61" t="s">
-        <v>478</v>
+        <v>490</v>
       </c>
       <c r="M54" s="61" t="n">
         <v>13.6</v>
       </c>
       <c r="N54" s="61" t="s">
-        <v>479</v>
+        <v>491</v>
       </c>
     </row>
     <row r="55" spans="1:18">
@@ -5136,43 +5184,43 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>480</v>
+        <v>492</v>
       </c>
       <c r="C55" s="61" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="D55" s="61" t="s">
         <v>31</v>
       </c>
       <c r="E55" s="61" t="s">
-        <v>432</v>
+        <v>442</v>
       </c>
       <c r="F55" s="32" t="s">
-        <v>481</v>
+        <v>493</v>
       </c>
       <c r="G55" s="61" t="s">
-        <v>482</v>
+        <v>494</v>
       </c>
       <c r="H55" s="61" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="I55" s="61" t="s">
-        <v>393</v>
+        <v>404</v>
       </c>
       <c r="J55" s="32" t="s">
-        <v>483</v>
+        <v>495</v>
       </c>
       <c r="K55" s="61" t="s">
-        <v>484</v>
+        <v>496</v>
       </c>
       <c r="L55" s="61" t="s">
-        <v>485</v>
+        <v>497</v>
       </c>
       <c r="M55" s="61" t="n">
         <v>13.4</v>
       </c>
       <c r="N55" s="61" t="s">
-        <v>486</v>
+        <v>498</v>
       </c>
     </row>
     <row r="56" spans="1:18">
@@ -5180,43 +5228,43 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>487</v>
+        <v>499</v>
       </c>
       <c r="C56" s="61" t="s">
-        <v>314</v>
+        <v>322</v>
       </c>
       <c r="D56" s="61" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="E56" s="61" t="s">
-        <v>488</v>
+        <v>500</v>
       </c>
       <c r="F56" s="32" t="s">
-        <v>325</v>
+        <v>333</v>
       </c>
       <c r="G56" s="61" t="s">
-        <v>489</v>
+        <v>501</v>
       </c>
       <c r="H56" s="61" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="I56" s="61" t="s">
-        <v>490</v>
+        <v>502</v>
       </c>
       <c r="J56" s="32" t="s">
-        <v>491</v>
+        <v>503</v>
       </c>
       <c r="K56" s="61" t="s">
-        <v>492</v>
+        <v>504</v>
       </c>
       <c r="L56" s="61" t="s">
-        <v>493</v>
+        <v>505</v>
       </c>
       <c r="M56" s="61" t="n">
         <v>13.5</v>
       </c>
       <c r="N56" s="61" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
     </row>
     <row r="57" spans="1:18">
@@ -5224,43 +5272,43 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>494</v>
+        <v>506</v>
       </c>
       <c r="C57" s="61" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="D57" s="61" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E57" s="61" t="s">
-        <v>495</v>
+        <v>507</v>
       </c>
       <c r="F57" s="32" t="s">
-        <v>496</v>
+        <v>508</v>
       </c>
       <c r="G57" s="61" t="s">
-        <v>497</v>
+        <v>509</v>
       </c>
       <c r="H57" s="61" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="I57" s="61" t="s">
-        <v>476</v>
+        <v>488</v>
       </c>
       <c r="J57" s="32" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="K57" s="61" t="s">
-        <v>498</v>
+        <v>510</v>
       </c>
       <c r="L57" s="61" t="s">
-        <v>499</v>
+        <v>511</v>
       </c>
       <c r="M57" s="61" t="n">
         <v>10.7</v>
       </c>
       <c r="N57" s="61" t="s">
-        <v>420</v>
+        <v>430</v>
       </c>
     </row>
     <row r="58" spans="1:18">
@@ -5268,43 +5316,43 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>500</v>
+        <v>512</v>
       </c>
       <c r="C58" s="61" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="D58" s="61" t="s">
-        <v>501</v>
+        <v>513</v>
       </c>
       <c r="E58" s="61" t="s">
-        <v>502</v>
+        <v>514</v>
       </c>
       <c r="F58" s="32" t="s">
-        <v>503</v>
+        <v>515</v>
       </c>
       <c r="G58" s="61" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="H58" s="61" t="s">
-        <v>504</v>
+        <v>516</v>
       </c>
       <c r="I58" s="61" t="s">
-        <v>505</v>
+        <v>517</v>
       </c>
       <c r="J58" s="32" t="s">
-        <v>506</v>
+        <v>518</v>
       </c>
       <c r="K58" s="61" t="s">
-        <v>507</v>
+        <v>519</v>
       </c>
       <c r="L58" s="61" t="s">
-        <v>508</v>
+        <v>520</v>
       </c>
       <c r="M58" s="61" t="n">
         <v>12.7</v>
       </c>
       <c r="N58" s="61" t="s">
-        <v>509</v>
+        <v>521</v>
       </c>
     </row>
     <row r="59" spans="1:18">
@@ -5312,43 +5360,43 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>510</v>
+        <v>522</v>
       </c>
       <c r="C59" s="61" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D59" s="61" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="E59" s="61" t="s">
-        <v>511</v>
+        <v>523</v>
       </c>
       <c r="F59" s="32" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G59" s="61" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="H59" s="61" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I59" s="61" t="s">
-        <v>512</v>
+        <v>524</v>
       </c>
       <c r="J59" s="32" t="s">
-        <v>513</v>
-      </c>
-      <c r="K59" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="L59" s="61" t="n">
-        <v>0</v>
+        <v>525</v>
+      </c>
+      <c r="K59" s="61" t="s">
+        <v>137</v>
+      </c>
+      <c r="L59" s="61" t="s">
+        <v>526</v>
       </c>
       <c r="M59" s="61" t="n">
-        <v>0</v>
+        <v>14.9</v>
       </c>
       <c r="N59" s="61" t="s">
-        <v>514</v>
+        <v>527</v>
       </c>
     </row>
     <row r="60" spans="1:18">
@@ -5356,43 +5404,43 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>515</v>
+        <v>528</v>
       </c>
       <c r="C60" s="61" t="s">
-        <v>482</v>
+        <v>494</v>
       </c>
       <c r="D60" s="61" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E60" s="61" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F60" s="32" t="s">
-        <v>516</v>
+        <v>529</v>
       </c>
       <c r="G60" s="61" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="H60" s="61" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="I60" s="61" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="J60" s="32" t="s">
-        <v>517</v>
+        <v>530</v>
       </c>
       <c r="K60" s="61" t="s">
-        <v>518</v>
+        <v>531</v>
       </c>
       <c r="L60" s="61" t="s">
-        <v>519</v>
+        <v>532</v>
       </c>
       <c r="M60" s="61" t="n">
         <v>13.1</v>
       </c>
       <c r="N60" s="61" t="s">
-        <v>520</v>
+        <v>533</v>
       </c>
     </row>
     <row r="61" spans="1:18">
@@ -5400,43 +5448,43 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>521</v>
+        <v>534</v>
       </c>
       <c r="C61" s="61" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D61" s="61" t="s">
-        <v>522</v>
+        <v>535</v>
       </c>
       <c r="E61" s="61" t="s">
-        <v>523</v>
+        <v>536</v>
       </c>
       <c r="F61" s="32" t="s">
-        <v>409</v>
+        <v>419</v>
       </c>
       <c r="G61" s="61" t="s">
-        <v>342</v>
+        <v>350</v>
       </c>
       <c r="H61" s="61" t="s">
-        <v>475</v>
+        <v>487</v>
       </c>
       <c r="I61" s="61" t="s">
-        <v>524</v>
+        <v>537</v>
       </c>
       <c r="J61" s="32" t="s">
-        <v>525</v>
+        <v>538</v>
       </c>
       <c r="K61" s="61" t="s">
-        <v>526</v>
+        <v>539</v>
       </c>
       <c r="L61" s="61" t="s">
-        <v>527</v>
+        <v>540</v>
       </c>
       <c r="M61" s="61" t="n">
         <v>12.4</v>
       </c>
       <c r="N61" s="61" t="s">
-        <v>528</v>
+        <v>541</v>
       </c>
     </row>
     <row r="62" spans="1:18">
@@ -5444,43 +5492,43 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>529</v>
+        <v>542</v>
       </c>
       <c r="C62" s="61" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D62" s="61" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E62" s="61" t="s">
-        <v>530</v>
+        <v>543</v>
       </c>
       <c r="F62" s="32" t="s">
-        <v>531</v>
+        <v>544</v>
       </c>
       <c r="G62" s="61" t="s">
         <v>34</v>
       </c>
       <c r="H62" s="61" t="s">
-        <v>532</v>
+        <v>545</v>
       </c>
       <c r="I62" s="61" t="s">
-        <v>300</v>
+        <v>306</v>
       </c>
       <c r="J62" s="32" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="K62" s="61" t="s">
-        <v>317</v>
+        <v>325</v>
       </c>
       <c r="L62" s="61" t="s">
-        <v>388</v>
+        <v>399</v>
       </c>
       <c r="M62" s="61" t="n">
         <v>10.5</v>
       </c>
       <c r="N62" s="61" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
     </row>
     <row r="63" spans="1:18">
@@ -5488,43 +5536,43 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>533</v>
+        <v>546</v>
       </c>
       <c r="C63" s="61" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D63" s="61" t="s">
         <v>35</v>
       </c>
       <c r="E63" s="61" t="s">
-        <v>534</v>
+        <v>547</v>
       </c>
       <c r="F63" s="32" t="s">
-        <v>325</v>
+        <v>333</v>
       </c>
       <c r="G63" s="61" t="s">
-        <v>535</v>
+        <v>548</v>
       </c>
       <c r="H63" s="61" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="I63" s="61" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="J63" s="32" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="K63" s="61" t="s">
-        <v>536</v>
+        <v>549</v>
       </c>
       <c r="L63" s="61" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="M63" s="61" t="n">
         <v>11.5</v>
       </c>
       <c r="N63" s="61" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
     </row>
     <row r="64" spans="1:18">
@@ -5532,43 +5580,43 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>537</v>
+        <v>550</v>
       </c>
       <c r="C64" s="61" t="s">
-        <v>538</v>
+        <v>551</v>
       </c>
       <c r="D64" s="61" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E64" s="61" t="s">
-        <v>539</v>
+        <v>552</v>
       </c>
       <c r="F64" s="32" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="G64" s="61" t="s">
-        <v>474</v>
+        <v>486</v>
       </c>
       <c r="H64" s="61" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="I64" s="61" t="s">
-        <v>540</v>
+        <v>553</v>
       </c>
       <c r="J64" s="32" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="K64" s="61" t="s">
-        <v>541</v>
+        <v>554</v>
       </c>
       <c r="L64" s="61" t="s">
-        <v>542</v>
+        <v>526</v>
       </c>
       <c r="M64" s="61" t="n">
         <v>11.5</v>
       </c>
       <c r="N64" s="61" t="s">
-        <v>543</v>
+        <v>555</v>
       </c>
     </row>
     <row r="65" spans="1:18">
@@ -5576,43 +5624,43 @@
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>544</v>
+        <v>556</v>
       </c>
       <c r="C65" s="61" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D65" s="61" t="s">
-        <v>545</v>
+        <v>557</v>
       </c>
       <c r="E65" s="61" t="s">
-        <v>546</v>
+        <v>558</v>
       </c>
       <c r="F65" s="32" t="s">
-        <v>547</v>
+        <v>559</v>
       </c>
       <c r="G65" s="61" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="H65" s="61" t="s">
-        <v>475</v>
+        <v>487</v>
       </c>
       <c r="I65" s="61" t="s">
-        <v>548</v>
+        <v>560</v>
       </c>
       <c r="J65" s="32" t="s">
-        <v>386</v>
-      </c>
-      <c r="K65" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="L65" s="61" t="n">
-        <v>0</v>
+        <v>397</v>
+      </c>
+      <c r="K65" s="61" t="s">
+        <v>561</v>
+      </c>
+      <c r="L65" s="61" t="s">
+        <v>562</v>
       </c>
       <c r="M65" s="61" t="n">
-        <v>0</v>
+        <v>12.4</v>
       </c>
       <c r="N65" s="61" t="s">
-        <v>549</v>
+        <v>563</v>
       </c>
     </row>
     <row r="66" spans="1:18">
@@ -5620,43 +5668,43 @@
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>550</v>
+        <v>564</v>
       </c>
       <c r="C66" s="61" t="s">
-        <v>314</v>
+        <v>322</v>
       </c>
       <c r="D66" s="61" t="s">
-        <v>551</v>
+        <v>565</v>
       </c>
       <c r="E66" s="61" t="s">
         <v>20</v>
       </c>
       <c r="F66" s="32" t="s">
-        <v>409</v>
+        <v>419</v>
       </c>
       <c r="G66" s="61" t="s">
-        <v>552</v>
+        <v>566</v>
       </c>
       <c r="H66" s="61" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="I66" s="61" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="J66" s="32" t="s">
-        <v>553</v>
-      </c>
-      <c r="K66" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="L66" s="61" t="n">
-        <v>0</v>
+        <v>567</v>
+      </c>
+      <c r="K66" s="61" t="s">
+        <v>568</v>
+      </c>
+      <c r="L66" s="61" t="s">
+        <v>569</v>
       </c>
       <c r="M66" s="61" t="n">
-        <v>0</v>
+        <v>10.2</v>
       </c>
       <c r="N66" s="61" t="s">
-        <v>554</v>
+        <v>570</v>
       </c>
     </row>
     <row r="67" spans="1:18">
@@ -5664,43 +5712,43 @@
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>555</v>
+        <v>571</v>
       </c>
       <c r="C67" s="61" t="s">
         <v>34</v>
       </c>
       <c r="D67" s="61" t="s">
-        <v>374</v>
+        <v>384</v>
       </c>
       <c r="E67" s="61" t="s">
-        <v>556</v>
+        <v>572</v>
       </c>
       <c r="F67" s="32" t="s">
-        <v>379</v>
+        <v>390</v>
       </c>
       <c r="G67" s="61" t="s">
-        <v>474</v>
+        <v>486</v>
       </c>
       <c r="H67" s="61" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="I67" s="61" t="s">
-        <v>548</v>
+        <v>560</v>
       </c>
       <c r="J67" s="32" t="s">
-        <v>467</v>
+        <v>479</v>
       </c>
       <c r="K67" s="61" t="s">
-        <v>557</v>
+        <v>573</v>
       </c>
       <c r="L67" s="61" t="s">
-        <v>508</v>
+        <v>520</v>
       </c>
       <c r="M67" s="61" t="n">
         <v>12.3</v>
       </c>
       <c r="N67" s="61" t="s">
-        <v>558</v>
+        <v>574</v>
       </c>
     </row>
     <row r="68" spans="1:18">
@@ -5708,43 +5756,43 @@
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>559</v>
+        <v>575</v>
       </c>
       <c r="C68" s="61" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D68" s="61" t="s">
-        <v>311</v>
+        <v>319</v>
       </c>
       <c r="E68" s="61" t="s">
-        <v>560</v>
+        <v>576</v>
       </c>
       <c r="F68" s="32" t="s">
-        <v>561</v>
+        <v>577</v>
       </c>
       <c r="G68" s="61" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H68" s="61" t="s">
-        <v>562</v>
+        <v>578</v>
       </c>
       <c r="I68" s="61" t="s">
-        <v>563</v>
+        <v>579</v>
       </c>
       <c r="J68" s="32" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="K68" s="61" t="s">
-        <v>407</v>
+        <v>417</v>
       </c>
       <c r="L68" s="61" t="s">
-        <v>564</v>
+        <v>580</v>
       </c>
       <c r="M68" s="61" t="n">
         <v>8.699999999999999</v>
       </c>
       <c r="N68" s="61" t="s">
-        <v>318</v>
+        <v>326</v>
       </c>
     </row>
     <row r="69" spans="1:18">
@@ -5752,43 +5800,43 @@
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>565</v>
+        <v>581</v>
       </c>
       <c r="C69" s="61" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D69" s="61" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="E69" s="61" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="F69" s="32" t="s">
-        <v>566</v>
+        <v>582</v>
       </c>
       <c r="G69" s="61" t="s">
-        <v>567</v>
+        <v>583</v>
       </c>
       <c r="H69" s="61" t="s">
-        <v>334</v>
+        <v>342</v>
       </c>
       <c r="I69" s="61" t="s">
-        <v>324</v>
+        <v>332</v>
       </c>
       <c r="J69" s="32" t="s">
-        <v>568</v>
+        <v>584</v>
       </c>
       <c r="K69" s="61" t="s">
-        <v>569</v>
+        <v>585</v>
       </c>
       <c r="L69" s="61" t="s">
-        <v>570</v>
+        <v>586</v>
       </c>
       <c r="M69" s="61" t="n">
         <v>14</v>
       </c>
       <c r="N69" s="61" t="s">
-        <v>571</v>
+        <v>587</v>
       </c>
     </row>
     <row r="70" spans="1:18">
@@ -5796,43 +5844,43 @@
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>572</v>
+        <v>588</v>
       </c>
       <c r="C70" s="61" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="D70" s="61" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="E70" s="61" t="s">
-        <v>573</v>
+        <v>589</v>
       </c>
       <c r="F70" s="32" t="s">
-        <v>574</v>
+        <v>590</v>
       </c>
       <c r="G70" s="61" t="s">
-        <v>348</v>
+        <v>356</v>
       </c>
       <c r="H70" s="61" t="s">
         <v>35</v>
       </c>
       <c r="I70" s="61" t="s">
-        <v>575</v>
+        <v>591</v>
       </c>
       <c r="J70" s="32" t="s">
-        <v>576</v>
+        <v>592</v>
       </c>
       <c r="K70" s="61" t="s">
-        <v>345</v>
+        <v>353</v>
       </c>
       <c r="L70" s="61" t="s">
-        <v>577</v>
+        <v>593</v>
       </c>
       <c r="M70" s="61" t="n">
         <v>10.4</v>
       </c>
       <c r="N70" s="61" t="s">
-        <v>578</v>
+        <v>594</v>
       </c>
     </row>
   </sheetData>
@@ -5869,12 +5917,12 @@
   <sheetData>
     <row r="1" spans="1:27">
       <c r="B1" t="s">
-        <v>579</v>
+        <v>595</v>
       </c>
     </row>
     <row r="2" spans="1:27">
       <c r="B2" s="3" t="s">
-        <v>580</v>
+        <v>596</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>4</v>
@@ -5970,7 +6018,7 @@
         <v/>
       </c>
       <c r="AA3" t="s">
-        <v>581</v>
+        <v>597</v>
       </c>
     </row>
     <row r="4" spans="1:27">
@@ -6167,7 +6215,7 @@
         <v/>
       </c>
       <c r="AA7" t="s">
-        <v>582</v>
+        <v>598</v>
       </c>
     </row>
     <row r="8" spans="1:27">
@@ -6244,7 +6292,7 @@
         <v/>
       </c>
       <c r="AA9" t="s">
-        <v>583</v>
+        <v>599</v>
       </c>
     </row>
     <row r="10" spans="1:27">
@@ -6440,7 +6488,7 @@
         <v/>
       </c>
       <c r="AA13" t="s">
-        <v>584</v>
+        <v>600</v>
       </c>
     </row>
     <row r="16" spans="1:27">
@@ -6476,12 +6524,12 @@
   <sheetData>
     <row r="1" spans="1:26">
       <c r="B1" t="s">
-        <v>585</v>
+        <v>601</v>
       </c>
     </row>
     <row r="2" spans="1:26">
       <c r="B2" s="3" t="s">
-        <v>580</v>
+        <v>596</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>4</v>
@@ -7592,7 +7640,7 @@
     </row>
     <row r="27" spans="1:26">
       <c r="B27" t="s">
-        <v>586</v>
+        <v>602</v>
       </c>
       <c r="D27" s="61" t="n"/>
       <c r="E27" s="61" t="n"/>
@@ -7607,7 +7655,7 @@
     </row>
     <row r="28" spans="1:26">
       <c r="B28" s="3" t="s">
-        <v>580</v>
+        <v>596</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>4</v>
@@ -8718,7 +8766,7 @@
     </row>
     <row r="53" spans="1:26">
       <c r="B53" t="s">
-        <v>587</v>
+        <v>603</v>
       </c>
       <c r="D53" s="61" t="n"/>
       <c r="E53" s="61" t="n"/>
@@ -8733,7 +8781,7 @@
     </row>
     <row r="54" spans="1:26">
       <c r="B54" s="3" t="s">
-        <v>580</v>
+        <v>596</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>4</v>
@@ -9842,7 +9890,7 @@
     </row>
     <row r="79" spans="1:26">
       <c r="B79" t="s">
-        <v>588</v>
+        <v>604</v>
       </c>
       <c r="D79" s="61" t="n"/>
       <c r="E79" s="61" t="n"/>
@@ -9857,7 +9905,7 @@
     </row>
     <row r="80" spans="1:26">
       <c r="B80" s="46" t="s">
-        <v>580</v>
+        <v>596</v>
       </c>
       <c r="C80" s="47" t="s">
         <v>4</v>
@@ -10685,7 +10733,7 @@
         <v/>
       </c>
       <c r="Z97" t="s">
-        <v>589</v>
+        <v>605</v>
       </c>
     </row>
     <row r="98" spans="1:26">
@@ -10995,12 +11043,12 @@
   <sheetData>
     <row r="1" spans="1:25">
       <c r="B1" t="s">
-        <v>585</v>
+        <v>601</v>
       </c>
     </row>
     <row r="2" spans="1:25">
       <c r="B2" s="3" t="s">
-        <v>580</v>
+        <v>596</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>4</v>
@@ -11837,7 +11885,7 @@
     </row>
     <row r="15" spans="1:25">
       <c r="B15" t="s">
-        <v>586</v>
+        <v>602</v>
       </c>
       <c r="D15" s="61" t="n"/>
       <c r="E15" s="61" t="n"/>
@@ -11852,7 +11900,7 @@
     </row>
     <row r="16" spans="1:25">
       <c r="B16" s="3" t="s">
-        <v>580</v>
+        <v>596</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>4</v>
@@ -12682,7 +12730,7 @@
     </row>
     <row r="29" spans="1:25">
       <c r="B29" t="s">
-        <v>587</v>
+        <v>603</v>
       </c>
       <c r="D29" s="61" t="n"/>
       <c r="E29" s="61" t="n"/>
@@ -12697,7 +12745,7 @@
     </row>
     <row r="30" spans="1:25">
       <c r="B30" s="3" t="s">
-        <v>580</v>
+        <v>596</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>4</v>
@@ -13536,7 +13584,7 @@
     </row>
     <row r="43" spans="1:25">
       <c r="B43" t="s">
-        <v>588</v>
+        <v>604</v>
       </c>
       <c r="D43" s="61" t="n"/>
       <c r="E43" s="61" t="n"/>
@@ -13551,7 +13599,7 @@
     </row>
     <row r="44" spans="1:25">
       <c r="B44" s="3" t="s">
-        <v>580</v>
+        <v>596</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>4</v>
@@ -14431,12 +14479,12 @@
   <sheetData>
     <row r="1" spans="1:25">
       <c r="B1" t="s">
-        <v>585</v>
+        <v>601</v>
       </c>
     </row>
     <row r="2" spans="1:25">
       <c r="B2" s="3" t="s">
-        <v>580</v>
+        <v>596</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>4</v>
@@ -14878,7 +14926,7 @@
     </row>
     <row r="9" spans="1:25">
       <c r="B9" t="s">
-        <v>586</v>
+        <v>602</v>
       </c>
       <c r="D9" s="61" t="n"/>
       <c r="E9" s="61" t="n"/>
@@ -14893,7 +14941,7 @@
     </row>
     <row r="10" spans="1:25">
       <c r="B10" s="3" t="s">
-        <v>580</v>
+        <v>596</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>4</v>
@@ -15335,7 +15383,7 @@
     </row>
     <row r="17" spans="1:25">
       <c r="B17" t="s">
-        <v>587</v>
+        <v>603</v>
       </c>
       <c r="D17" s="61" t="n"/>
       <c r="E17" s="61" t="n"/>
@@ -15350,7 +15398,7 @@
     </row>
     <row r="18" spans="1:25">
       <c r="B18" s="3" t="s">
-        <v>580</v>
+        <v>596</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>4</v>
@@ -15792,7 +15840,7 @@
     </row>
     <row r="25" spans="1:25">
       <c r="B25" t="s">
-        <v>588</v>
+        <v>604</v>
       </c>
       <c r="D25" s="61" t="n"/>
       <c r="E25" s="61" t="n"/>
@@ -15807,7 +15855,7 @@
     </row>
     <row r="26" spans="1:25">
       <c r="B26" s="3" t="s">
-        <v>580</v>
+        <v>596</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>4</v>
@@ -16270,12 +16318,12 @@
   <sheetData>
     <row r="1" spans="1:25">
       <c r="B1" t="s">
-        <v>585</v>
+        <v>601</v>
       </c>
     </row>
     <row r="2" spans="1:25">
       <c r="B2" s="3" t="s">
-        <v>580</v>
+        <v>596</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>4</v>
@@ -16515,7 +16563,7 @@
     </row>
     <row r="6" spans="1:25">
       <c r="B6" t="s">
-        <v>586</v>
+        <v>602</v>
       </c>
       <c r="D6" s="61" t="n"/>
       <c r="E6" s="61" t="n"/>
@@ -16530,7 +16578,7 @@
     </row>
     <row r="7" spans="1:25">
       <c r="B7" s="3" t="s">
-        <v>580</v>
+        <v>596</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>4</v>
@@ -16770,7 +16818,7 @@
     </row>
     <row r="11" spans="1:25">
       <c r="B11" t="s">
-        <v>587</v>
+        <v>603</v>
       </c>
       <c r="D11" s="61" t="n"/>
       <c r="E11" s="61" t="n"/>
@@ -16785,7 +16833,7 @@
     </row>
     <row r="12" spans="1:25">
       <c r="B12" s="3" t="s">
-        <v>580</v>
+        <v>596</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>4</v>
@@ -17025,7 +17073,7 @@
     </row>
     <row r="16" spans="1:25">
       <c r="B16" t="s">
-        <v>588</v>
+        <v>604</v>
       </c>
       <c r="D16" s="61" t="n"/>
       <c r="E16" s="61" t="n"/>
@@ -17040,7 +17088,7 @@
     </row>
     <row r="17" spans="1:25">
       <c r="B17" s="3" t="s">
-        <v>580</v>
+        <v>596</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>4</v>
@@ -17289,12 +17337,12 @@
   <sheetData>
     <row r="1" spans="1:25">
       <c r="B1" t="s">
-        <v>590</v>
+        <v>606</v>
       </c>
     </row>
     <row r="2" spans="1:25">
       <c r="B2" s="3" t="s">
-        <v>580</v>
+        <v>596</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>4</v>
@@ -17534,7 +17582,7 @@
     </row>
     <row r="6" spans="1:25">
       <c r="B6" t="s">
-        <v>591</v>
+        <v>607</v>
       </c>
       <c r="D6" s="61" t="n"/>
       <c r="E6" s="61" t="n"/>
@@ -17549,7 +17597,7 @@
     </row>
     <row r="7" spans="1:25">
       <c r="B7" s="3" t="s">
-        <v>580</v>
+        <v>596</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>4</v>
@@ -17817,7 +17865,7 @@
   <sheetData>
     <row r="4" spans="1:25">
       <c r="B4" s="3" t="s">
-        <v>580</v>
+        <v>596</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>4</v>
@@ -18057,7 +18105,7 @@
     </row>
     <row r="9" spans="1:25">
       <c r="L9" s="20" t="s">
-        <v>592</v>
+        <v>608</v>
       </c>
       <c r="M9">
         <f>IF(Y5&gt;Y6,C5,C6)</f>
@@ -18090,43 +18138,43 @@
   <sheetData>
     <row r="2" spans="1:15">
       <c r="B2" t="s">
-        <v>593</v>
+        <v>609</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>594</v>
+        <v>610</v>
       </c>
       <c r="E2" t="n">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>595</v>
+        <v>611</v>
       </c>
       <c r="G2" t="n">
         <v>4</v>
       </c>
       <c r="H2" t="s">
-        <v>596</v>
+        <v>612</v>
       </c>
       <c r="I2" t="n">
         <v>3</v>
       </c>
       <c r="J2" t="s">
-        <v>597</v>
+        <v>613</v>
       </c>
       <c r="K2" t="n">
         <v>0</v>
       </c>
       <c r="L2" t="s">
-        <v>598</v>
+        <v>614</v>
       </c>
       <c r="M2" t="n">
         <v>2</v>
       </c>
       <c r="N2" t="s">
-        <v>599</v>
+        <v>615</v>
       </c>
       <c r="O2">
         <f>SUM(C2+E2+G2+I2+K2+M2)</f>
@@ -18135,43 +18183,43 @@
     </row>
     <row r="3" spans="1:15">
       <c r="B3" t="s">
-        <v>600</v>
+        <v>616</v>
       </c>
       <c r="C3" t="n">
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>600</v>
+        <v>616</v>
       </c>
       <c r="E3" t="n">
         <v>4</v>
       </c>
       <c r="F3" t="s">
-        <v>600</v>
+        <v>616</v>
       </c>
       <c r="G3" t="n">
         <v>6</v>
       </c>
       <c r="H3" t="s">
-        <v>600</v>
+        <v>616</v>
       </c>
       <c r="I3" t="n">
         <v>3</v>
       </c>
       <c r="J3" t="s">
-        <v>600</v>
+        <v>616</v>
       </c>
       <c r="K3" t="n">
         <v>1</v>
       </c>
       <c r="L3" t="s">
-        <v>600</v>
+        <v>616</v>
       </c>
       <c r="M3" t="n">
         <v>2</v>
       </c>
       <c r="N3" t="s">
-        <v>600</v>
+        <v>616</v>
       </c>
       <c r="O3">
         <f>SUM(C3+E3+G3+I3+K3+M3)</f>
@@ -18180,49 +18228,49 @@
     </row>
     <row r="4" spans="1:15">
       <c r="B4" t="s">
-        <v>601</v>
+        <v>617</v>
       </c>
       <c r="C4" s="41">
         <f>C2/C3</f>
         <v/>
       </c>
       <c r="D4" t="s">
-        <v>601</v>
+        <v>617</v>
       </c>
       <c r="E4" s="41">
         <f>E2/E3</f>
         <v/>
       </c>
       <c r="F4" t="s">
-        <v>601</v>
+        <v>617</v>
       </c>
       <c r="G4" s="41">
         <f>G2/G3</f>
         <v/>
       </c>
       <c r="H4" t="s">
-        <v>601</v>
+        <v>617</v>
       </c>
       <c r="I4" s="41">
         <f>I2/I3</f>
         <v/>
       </c>
       <c r="J4" t="s">
-        <v>601</v>
+        <v>617</v>
       </c>
       <c r="K4" s="41">
         <f>K2/K3</f>
         <v/>
       </c>
       <c r="L4" t="s">
-        <v>601</v>
+        <v>617</v>
       </c>
       <c r="M4" s="41">
         <f>M2/M3</f>
         <v/>
       </c>
       <c r="N4" t="s">
-        <v>601</v>
+        <v>617</v>
       </c>
       <c r="O4" s="81">
         <f>O2/O3</f>

</xml_diff>